<commit_message>
tabelas e modelagem atualizada, criei routes, controllers and models
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E6C9FF-C113-402E-AD66-06EB9156420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A81D5-63C6-47C9-A1E0-E183A85C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3212,8 +3212,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update nas fotos do bd
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F634AF-C973-4743-9742-3DC36D042256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D26310-0C42-4744-81BC-7EAB6968F64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3048" yWindow="2196" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="1" r:id="rId1"/>
@@ -1861,10 +1861,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>249</c:v>
+                  <c:v>301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>108</c:v>
@@ -3212,8 +3212,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3331,11 +3331,11 @@
       </c>
       <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>249</v>
+        <v>301</v>
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="P3" s="41">
         <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&lt;="&amp;N3,$J$2:$J$44,TRUE))</f>
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="Q3" s="42">
         <f>O3-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N3,$J$2:$J$44,TRUE)))</f>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="Q5" s="39">
         <f>O5-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N5,$J$2:$J$44,TRUE)))</f>
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="Q6" s="37">
         <f>O6-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N6,$J$2:$J$44,TRUE)))</f>
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -3596,11 +3596,11 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" ref="P7:Q7" si="2">AVERAGE(P3:P6)</f>
-        <v>62.25</v>
+        <v>75.25</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="2"/>
-        <v>33.25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -4206,11 +4206,13 @@
       <c r="I23" s="21">
         <v>45978</v>
       </c>
-      <c r="J23" s="52" t="str">
+      <c r="J23" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K23" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="51">
+        <v>45963</v>
+      </c>
       <c r="L23" s="31" t="b">
         <v>0</v>
       </c>
@@ -4227,7 +4229,7 @@
         <v>46</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>20</v>
@@ -4314,11 +4316,13 @@
       <c r="I26" s="13">
         <v>45985</v>
       </c>
-      <c r="J26" s="52" t="str">
+      <c r="J26" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K26" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="50">
+        <v>45963</v>
+      </c>
       <c r="L26" s="30" t="b">
         <v>0</v>
       </c>
@@ -4578,11 +4582,13 @@
       <c r="I33" s="21">
         <v>45978</v>
       </c>
-      <c r="J33" s="52" t="str">
+      <c r="J33" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K33" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K33" s="51">
+        <v>45962</v>
+      </c>
       <c r="L33" s="31" t="b">
         <v>0</v>
       </c>
@@ -4614,11 +4620,13 @@
       <c r="I34" s="13">
         <v>45978</v>
       </c>
-      <c r="J34" s="52" t="str">
+      <c r="J34" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K34" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="50">
+        <v>45963</v>
+      </c>
       <c r="L34" s="30" t="b">
         <v>0</v>
       </c>
@@ -4650,11 +4658,13 @@
       <c r="I35" s="21">
         <v>45985</v>
       </c>
-      <c r="J35" s="52" t="str">
+      <c r="J35" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K35" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="51">
+        <v>45963</v>
+      </c>
       <c r="L35" s="31" t="b">
         <v>0</v>
       </c>
@@ -4956,11 +4966,13 @@
       <c r="I43" s="21">
         <v>45985</v>
       </c>
-      <c r="J43" s="52" t="str">
+      <c r="J43" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K43" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K43" s="51">
+        <v>45995</v>
+      </c>
       <c r="L43" s="31" t="b">
         <v>0</v>
       </c>
@@ -4992,11 +5004,13 @@
       <c r="I44" s="13">
         <v>45985</v>
       </c>
-      <c r="J44" s="52" t="str">
+      <c r="J44" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K44" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K44" s="50">
+        <v>45995</v>
+      </c>
       <c r="L44" s="30" t="b">
         <v>0</v>
       </c>

</xml_diff>